<commit_message>
22.07.2018_Commit after including the Bundled related Scenarios
</commit_message>
<xml_diff>
--- a/Resources/Data/Data.xlsx
+++ b/Resources/Data/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="672">
   <si>
     <t>S.No</t>
   </si>
@@ -2084,6 +2084,9 @@
   </si>
   <si>
     <t xml:space="preserve">V_83697                 </t>
+  </si>
+  <si>
+    <t>2001712</t>
   </si>
 </sst>
 </file>
@@ -2396,7 +2399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2555,11 +2558,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4F6228"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3281,34 +3293,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:F3">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:K3">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",L3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",M3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",M3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3322,7 +3334,7 @@
   <dimension ref="A1:L217"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M140" sqref="M140"/>
+      <selection activeCell="M199" sqref="M199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8243,8 +8255,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130" s="30" t="s">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="60" t="s">
         <v>319</v>
       </c>
       <c r="B130" s="31" t="s">
@@ -8281,8 +8293,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A131" s="30" t="s">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="60" t="s">
         <v>320</v>
       </c>
       <c r="B131" s="31" t="s">
@@ -8319,8 +8331,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="s">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="60" t="s">
         <v>321</v>
       </c>
       <c r="B132" s="31" t="s">
@@ -8357,8 +8369,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A133" s="30" t="s">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="60" t="s">
         <v>322</v>
       </c>
       <c r="B133" s="31" t="s">
@@ -8395,8 +8407,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A134" s="30" t="s">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="60" t="s">
         <v>323</v>
       </c>
       <c r="B134" s="31" t="s">
@@ -8433,8 +8445,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A135" s="30" t="s">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="60" t="s">
         <v>324</v>
       </c>
       <c r="B135" s="31" t="s">
@@ -8471,8 +8483,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="s">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="60" t="s">
         <v>325</v>
       </c>
       <c r="B136" s="31" t="s">
@@ -8509,8 +8521,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A137" s="30" t="s">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="60" t="s">
         <v>326</v>
       </c>
       <c r="B137" s="31" t="s">
@@ -8547,8 +8559,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A138" s="30" t="s">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="60" t="s">
         <v>327</v>
       </c>
       <c r="B138" s="31" t="s">
@@ -8585,8 +8597,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A139" s="30" t="s">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="60" t="s">
         <v>328</v>
       </c>
       <c r="B139" s="31" t="s">
@@ -8623,8 +8635,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A140" s="30" t="s">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="60" t="s">
         <v>329</v>
       </c>
       <c r="B140" s="31" t="s">
@@ -8661,8 +8673,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A141" s="30" t="s">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="60" t="s">
         <v>330</v>
       </c>
       <c r="B141" s="31" t="s">
@@ -8699,8 +8711,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A142" s="30" t="s">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="60" t="s">
         <v>331</v>
       </c>
       <c r="B142" s="31" t="s">
@@ -8737,8 +8749,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A143" s="30" t="s">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="60" t="s">
         <v>333</v>
       </c>
       <c r="B143" s="31" t="s">
@@ -8775,8 +8787,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A144" s="30" t="s">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="60" t="s">
         <v>334</v>
       </c>
       <c r="B144" s="31" t="s">
@@ -8813,8 +8825,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A145" s="30" t="s">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="60" t="s">
         <v>335</v>
       </c>
       <c r="B145" s="31" t="s">
@@ -8851,8 +8863,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A146" s="30" t="s">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="60" t="s">
         <v>336</v>
       </c>
       <c r="B146" s="31" t="s">
@@ -8889,8 +8901,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" s="30" t="s">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="60" t="s">
         <v>337</v>
       </c>
       <c r="B147" s="31" t="s">
@@ -10827,7 +10839,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="30" t="s">
         <v>518</v>
       </c>
@@ -10838,7 +10850,7 @@
         <v>231</v>
       </c>
       <c r="D198" s="32" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E198" s="33" t="s">
         <v>48</v>
@@ -10859,13 +10871,13 @@
         <v>78</v>
       </c>
       <c r="K198" s="34" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L198" s="37" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="199" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="30" t="s">
         <v>520</v>
       </c>
@@ -10903,7 +10915,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="200" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="30" t="s">
         <v>522</v>
       </c>
@@ -10941,7 +10953,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="201" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="30" t="s">
         <v>524</v>
       </c>
@@ -10979,7 +10991,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="202" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="30" t="s">
         <v>526</v>
       </c>
@@ -11017,7 +11029,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="30" t="s">
         <v>528</v>
       </c>
@@ -11055,7 +11067,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="30" t="s">
         <v>530</v>
       </c>
@@ -11093,7 +11105,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="30" t="s">
         <v>532</v>
       </c>
@@ -11131,7 +11143,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="206" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="30" t="s">
         <v>534</v>
       </c>
@@ -11169,7 +11181,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="207" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="30" t="s">
         <v>536</v>
       </c>
@@ -11207,7 +11219,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="208" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="30" t="s">
         <v>538</v>
       </c>
@@ -11245,7 +11257,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="209" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="30" t="s">
         <v>540</v>
       </c>
@@ -11283,7 +11295,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="210" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="30" t="s">
         <v>542</v>
       </c>
@@ -11321,7 +11333,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="211" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="30" t="s">
         <v>544</v>
       </c>
@@ -11359,7 +11371,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="30" t="s">
         <v>546</v>
       </c>
@@ -11397,7 +11409,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="30" t="s">
         <v>548</v>
       </c>
@@ -11435,7 +11447,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="30" t="s">
         <v>550</v>
       </c>
@@ -11473,7 +11485,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="215" spans="1:12" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="30" t="s">
         <v>552</v>
       </c>
@@ -11591,20 +11603,20 @@
   <autoFilter ref="C1:C217">
     <filterColumn colId="0">
       <filters>
-        <filter val="po order"/>
+        <filter val="petco_bundle sku"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="J1">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1 J218:J1048576 I2:I5">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11625,8 +11637,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P169"/>
   <sheetViews>
-    <sheetView topLeftCell="C142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H157" sqref="H157"/>
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14379,8 +14391,8 @@
       <c r="A59" s="41" t="s">
         <v>232</v>
       </c>
-      <c r="B59" s="63" t="s">
-        <v>230</v>
+      <c r="B59" s="66" t="s">
+        <v>671</v>
       </c>
       <c r="C59" s="41" t="s">
         <v>46</v>

</xml_diff>